<commit_message>
First density plots for SDD and gut transit time; Santa Maria missing
</commit_message>
<xml_diff>
--- a/Data/Seed_dispersal/Raw_TaquaraAnne_EMZ4_Seed-dispersal.xlsx
+++ b/Data/Seed_dispersal/Raw_TaquaraAnne_EMZ4_Seed-dispersal.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documentos\github\BLT_IBM-Model\Data\Seed_dispersal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7914984-FB1D-498A-B890-E406540B867C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D20C53E-472F-4503-AEA1-2520DA2CC72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw_TaquaraAnne_EMZ4_Seed-dispe" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Raw_TaquaraAnne_EMZ4_Seed-dispe'!$A$1:$L$151</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -2991,7 +2994,7 @@
         <v>65</v>
       </c>
       <c r="G32" s="1">
-        <v>43130.371527777781</v>
+        <v>43131.371527777781</v>
       </c>
       <c r="H32">
         <v>-52.247969740000002</v>
@@ -3029,7 +3032,7 @@
         <v>65</v>
       </c>
       <c r="G33" s="1">
-        <v>43130.378472222219</v>
+        <v>43131.378472222219</v>
       </c>
       <c r="H33">
         <v>-52.247070190000002</v>
@@ -3219,7 +3222,7 @@
         <v>68</v>
       </c>
       <c r="G38" s="1">
-        <v>43130.732638888891</v>
+        <v>43131.732638888891</v>
       </c>
       <c r="H38">
         <v>-52.248911130000003</v>
@@ -5651,7 +5654,7 @@
         <v>157</v>
       </c>
       <c r="G102" s="1">
-        <v>43283.361111111109</v>
+        <v>43284.361111111109</v>
       </c>
       <c r="H102">
         <v>-52.249048960000003</v>
@@ -5689,7 +5692,7 @@
         <v>157</v>
       </c>
       <c r="G103" s="1">
-        <v>43283.371527777781</v>
+        <v>43284.371527777781</v>
       </c>
       <c r="H103">
         <v>-52.248395389999999</v>
@@ -6297,7 +6300,7 @@
         <v>189</v>
       </c>
       <c r="G119" s="1">
-        <v>43360.34375</v>
+        <v>43361.34375</v>
       </c>
       <c r="H119">
         <v>-52.251927590000001</v>
@@ -6335,7 +6338,7 @@
         <v>190</v>
       </c>
       <c r="G120" s="1">
-        <v>43360.34375</v>
+        <v>43361.34375</v>
       </c>
       <c r="H120">
         <v>-52.251927590000001</v>
@@ -7532,6 +7535,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L151" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filtered movement data to match siminputrow matrix
</commit_message>
<xml_diff>
--- a/Data/Seed_dispersal/Raw_TaquaraAnne_EMZ4_Seed-dispersal.xlsx
+++ b/Data/Seed_dispersal/Raw_TaquaraAnne_EMZ4_Seed-dispersal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documentos\github\BLT_IBM-Model\Data\Seed_dispersal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8F83AD-0C43-4947-81AD-FDD8DE282D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD8C3B6-713E-4DE5-9225-7C28A8D6D4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,24 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Raw_TaquaraAnne_EMZ4_Seed-dispe'!$A$1:$M$151</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="309">
   <si>
     <t>id_feces</t>
   </si>
@@ -941,9 +953,6 @@
   </si>
   <si>
     <t>Dec2017</t>
-  </si>
-  <si>
-    <t>Feb</t>
   </si>
   <si>
     <t>May</t>
@@ -3399,7 +3408,7 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D39" s="1">
         <v>43132.302083333336</v>
@@ -3440,7 +3449,7 @@
         <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D40" s="1">
         <v>43132.3125</v>
@@ -3481,7 +3490,7 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D41" s="1">
         <v>43132.392361111109</v>
@@ -3522,7 +3531,7 @@
         <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D42" s="1">
         <v>43132.392361111109</v>
@@ -3563,7 +3572,7 @@
         <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D43" s="1">
         <v>43132.451388888891</v>
@@ -3604,7 +3613,7 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D44" s="1">
         <v>43132.451388888891</v>
@@ -3645,7 +3654,7 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D45" s="1">
         <v>43132.579861111109</v>
@@ -3686,7 +3695,7 @@
         <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D46" s="1">
         <v>43133.395833333336</v>
@@ -3727,7 +3736,7 @@
         <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D47" s="1">
         <v>43133.395833333336</v>
@@ -3768,7 +3777,7 @@
         <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D48" s="1">
         <v>43133.413194444445</v>
@@ -3809,7 +3818,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D49" s="1">
         <v>43133.413194444445</v>
@@ -3850,7 +3859,7 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D50" s="1">
         <v>43133.753472222219</v>
@@ -3891,7 +3900,7 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D51" s="1">
         <v>43134.298611111109</v>
@@ -3932,7 +3941,7 @@
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D52" s="1">
         <v>43135.305555555555</v>
@@ -3973,7 +3982,7 @@
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D53" s="1">
         <v>43134.309027777781</v>
@@ -4014,7 +4023,7 @@
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D54" s="1">
         <v>43135.559027777781</v>
@@ -4055,7 +4064,7 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D55" s="1">
         <v>43135.559027777781</v>
@@ -4096,7 +4105,7 @@
         <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D56" s="1">
         <v>43135.586805555555</v>
@@ -4137,7 +4146,7 @@
         <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D57" s="1">
         <v>43135.586805555555</v>
@@ -4178,7 +4187,7 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D58" s="1">
         <v>43159.430555555555</v>
@@ -4219,7 +4228,7 @@
         <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D59" s="1">
         <v>43159.430555555555</v>
@@ -4260,7 +4269,7 @@
         <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D60" s="1">
         <v>43159.440972222219</v>
@@ -4301,7 +4310,7 @@
         <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D61" s="1">
         <v>43159.440972222219</v>
@@ -4342,7 +4351,7 @@
         <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D62" s="1">
         <v>43159.65625</v>
@@ -4383,7 +4392,7 @@
         <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D63" s="1">
         <v>43159.65625</v>
@@ -4424,7 +4433,7 @@
         <v>35</v>
       </c>
       <c r="C64" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D64" s="1">
         <v>43159.6875</v>
@@ -4465,7 +4474,7 @@
         <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D65" s="1">
         <v>43159.6875</v>
@@ -4998,7 +5007,7 @@
         <v>78</v>
       </c>
       <c r="C78" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D78" s="1">
         <v>43222.371527777781</v>
@@ -5039,7 +5048,7 @@
         <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D79" s="1">
         <v>43222.465277777781</v>
@@ -5080,7 +5089,7 @@
         <v>75</v>
       </c>
       <c r="C80" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D80" s="1">
         <v>43222.756944444445</v>
@@ -5121,7 +5130,7 @@
         <v>75</v>
       </c>
       <c r="C81" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D81" s="1">
         <v>43222.756944444445</v>
@@ -5162,7 +5171,7 @@
         <v>75</v>
       </c>
       <c r="C82" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D82" s="1">
         <v>43222.756944444445</v>
@@ -5203,7 +5212,7 @@
         <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D83" s="1">
         <v>43223.274305555555</v>
@@ -5244,7 +5253,7 @@
         <v>78</v>
       </c>
       <c r="C84" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D84" s="1">
         <v>43223.274305555555</v>
@@ -5285,7 +5294,7 @@
         <v>78</v>
       </c>
       <c r="C85" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D85" s="1">
         <v>43223.274305555555</v>
@@ -5326,7 +5335,7 @@
         <v>78</v>
       </c>
       <c r="C86" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D86" s="1">
         <v>43223.274305555555</v>
@@ -5367,7 +5376,7 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D87" s="1">
         <v>43223.430555555555</v>
@@ -5408,7 +5417,7 @@
         <v>89</v>
       </c>
       <c r="C88" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D88" s="1">
         <v>43223.430555555555</v>
@@ -5449,7 +5458,7 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D89" s="1">
         <v>43223.447916666664</v>
@@ -5490,7 +5499,7 @@
         <v>91</v>
       </c>
       <c r="C90" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D90" s="1">
         <v>43223.447916666664</v>
@@ -5531,7 +5540,7 @@
         <v>61</v>
       </c>
       <c r="C91" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D91" s="1">
         <v>43223.569444444445</v>
@@ -5572,7 +5581,7 @@
         <v>61</v>
       </c>
       <c r="C92" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D92" s="1">
         <v>43223.569444444445</v>
@@ -5613,7 +5622,7 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D93" s="1">
         <v>43223.597222222219</v>
@@ -5654,7 +5663,7 @@
         <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D94" s="1">
         <v>43223.597222222219</v>
@@ -6351,7 +6360,7 @@
         <v>116</v>
       </c>
       <c r="C111" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D111" s="1">
         <v>43359.402777777781</v>
@@ -6392,7 +6401,7 @@
         <v>116</v>
       </c>
       <c r="C112" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D112" s="1">
         <v>43359.402777777781</v>
@@ -6433,7 +6442,7 @@
         <v>108</v>
       </c>
       <c r="C113" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D113" s="1">
         <v>43359.520833333336</v>
@@ -6474,7 +6483,7 @@
         <v>108</v>
       </c>
       <c r="C114" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D114" s="1">
         <v>43359.520833333336</v>
@@ -6515,7 +6524,7 @@
         <v>116</v>
       </c>
       <c r="C115" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D115" s="1">
         <v>43359.53125</v>
@@ -6556,7 +6565,7 @@
         <v>116</v>
       </c>
       <c r="C116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D116" s="1">
         <v>43359.53125</v>
@@ -6597,7 +6606,7 @@
         <v>108</v>
       </c>
       <c r="C117" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D117" s="1">
         <v>43360.506944444445</v>
@@ -6638,7 +6647,7 @@
         <v>108</v>
       </c>
       <c r="C118" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D118" s="1">
         <v>43360.506944444445</v>
@@ -6679,7 +6688,7 @@
         <v>111</v>
       </c>
       <c r="C119" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D119" s="1">
         <v>43360.65625</v>
@@ -6720,7 +6729,7 @@
         <v>80</v>
       </c>
       <c r="C120" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D120" s="1">
         <v>43360.666666666664</v>
@@ -6761,7 +6770,7 @@
         <v>95</v>
       </c>
       <c r="C121" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D121" s="1">
         <v>43361.357638888891</v>
@@ -6802,7 +6811,7 @@
         <v>95</v>
       </c>
       <c r="C122" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D122" s="1">
         <v>43361.357638888891</v>
@@ -6843,7 +6852,7 @@
         <v>95</v>
       </c>
       <c r="C123" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D123" s="1">
         <v>43361.357638888891</v>
@@ -6884,7 +6893,7 @@
         <v>108</v>
       </c>
       <c r="C124" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D124" s="1">
         <v>43361.524305555555</v>
@@ -6925,7 +6934,7 @@
         <v>108</v>
       </c>
       <c r="C125" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D125" s="1">
         <v>43361.524305555555</v>
@@ -6966,7 +6975,7 @@
         <v>111</v>
       </c>
       <c r="C126" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D126" s="1">
         <v>43362.361111111109</v>
@@ -7007,7 +7016,7 @@
         <v>111</v>
       </c>
       <c r="C127" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D127" s="1">
         <v>43362.361111111109</v>
@@ -7048,7 +7057,7 @@
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D128" s="1">
         <v>43362.371527777781</v>
@@ -7089,7 +7098,7 @@
         <v>130</v>
       </c>
       <c r="C129" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D129" s="1">
         <v>43362.371527777781</v>
@@ -7130,7 +7139,7 @@
         <v>95</v>
       </c>
       <c r="C130" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D130" s="1">
         <v>43362.392361111109</v>
@@ -7171,7 +7180,7 @@
         <v>111</v>
       </c>
       <c r="C131" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D131" s="1">
         <v>43362.46875</v>
@@ -7786,7 +7795,7 @@
         <v>18</v>
       </c>
       <c r="C146" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D146" s="1">
         <v>43435.319444444445</v>
@@ -7827,7 +7836,7 @@
         <v>18</v>
       </c>
       <c r="C147" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D147" s="1">
         <v>43435.319444444445</v>
@@ -7868,7 +7877,7 @@
         <v>148</v>
       </c>
       <c r="C148" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D148" s="1">
         <v>43435.385416666664</v>
@@ -7909,7 +7918,7 @@
         <v>148</v>
       </c>
       <c r="C149" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D149" s="1">
         <v>43435.385416666664</v>
@@ -7950,7 +7959,7 @@
         <v>25</v>
       </c>
       <c r="C150" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D150" s="1">
         <v>43435.399305555555</v>
@@ -7991,7 +8000,7 @@
         <v>25</v>
       </c>
       <c r="C151" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D151" s="1">
         <v>43435.399305555555</v>

</xml_diff>